<commit_message>
Update backedn proccess for bulk util and Db o[erations for Movies data ingestor
</commit_message>
<xml_diff>
--- a/templates/movie_bulk_upload_template.xlsx
+++ b/templates/movie_bulk_upload_template.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,6 +514,16 @@
           <t>budget</t>
         </is>
       </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>is_available</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -590,6 +600,14 @@
       <c r="P2" t="n">
         <v>63</v>
       </c>
+      <c r="Q2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>/movies/the_matrix.mp4</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -666,6 +684,14 @@
       <c r="P3" t="n">
         <v>70</v>
       </c>
+      <c r="Q3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>/movies/dangal.mp4</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -742,6 +768,14 @@
       <c r="P4" t="n">
         <v>356</v>
       </c>
+      <c r="Q4" t="b">
+        <v>1</v>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>/movies/avengers_endgame.mp4</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -818,6 +852,14 @@
       <c r="P5" t="n">
         <v>55</v>
       </c>
+      <c r="Q5" t="b">
+        <v>1</v>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>/movies/3_idiots.mp4</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -894,6 +936,10 @@
       <c r="P6" t="n">
         <v>11</v>
       </c>
+      <c r="Q6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>